<commit_message>
AKS - Bara mockup kvar nu.
</commit_message>
<xml_diff>
--- a/Kebab - Dataexempel.xlsx
+++ b/Kebab - Dataexempel.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="12075"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
   <si>
     <t>Maträtt</t>
   </si>
@@ -67,14 +67,150 @@
   </si>
   <si>
     <t>SpecialID</t>
+  </si>
+  <si>
+    <t>Kebabrulle</t>
+  </si>
+  <si>
+    <t>Kebabtalrik</t>
+  </si>
+  <si>
+    <t>Kebab i bröd</t>
+  </si>
+  <si>
+    <t>Stora salen</t>
+  </si>
+  <si>
+    <t>Lilla salen</t>
+  </si>
+  <si>
+    <t>Bokning</t>
+  </si>
+  <si>
+    <t>PatientID</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Tidsåtgång</t>
+  </si>
+  <si>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>Avlidit</t>
+  </si>
+  <si>
+    <t>Dödsruna</t>
+  </si>
+  <si>
+    <t>Ulf</t>
+  </si>
+  <si>
+    <t>Nisse</t>
+  </si>
+  <si>
+    <t>Tore</t>
+  </si>
+  <si>
+    <t>Gunnar</t>
+  </si>
+  <si>
+    <t>Legolas</t>
+  </si>
+  <si>
+    <t>Rudolfsson</t>
+  </si>
+  <si>
+    <t>Ahlsson</t>
+  </si>
+  <si>
+    <t>Olsson</t>
+  </si>
+  <si>
+    <t>Nilsson</t>
+  </si>
+  <si>
+    <t>Frodosson</t>
+  </si>
+  <si>
+    <t>Storgatan 1</t>
+  </si>
+  <si>
+    <t>Lillgatan 2</t>
+  </si>
+  <si>
+    <t>Halvgatan 13</t>
+  </si>
+  <si>
+    <t>Helgatan 22</t>
+  </si>
+  <si>
+    <t>123 45</t>
+  </si>
+  <si>
+    <t>123 46</t>
+  </si>
+  <si>
+    <t>123 33</t>
+  </si>
+  <si>
+    <t>123 82</t>
+  </si>
+  <si>
+    <t>111 11</t>
+  </si>
+  <si>
+    <t>Gandalfgatan 1</t>
+  </si>
+  <si>
+    <t>Kalmar</t>
+  </si>
+  <si>
+    <t>Fylke</t>
+  </si>
+  <si>
+    <t>580101-5068</t>
+  </si>
+  <si>
+    <t>180225-1234</t>
+  </si>
+  <si>
+    <t>990413-9876</t>
+  </si>
+  <si>
+    <t>861122-1010</t>
+  </si>
+  <si>
+    <t>530912-4320</t>
+  </si>
+  <si>
+    <t>Han ångrade ingenting.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -90,7 +226,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -98,18 +234,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -188,6 +373,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -222,6 +408,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -397,110 +584,495 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="A16" sqref="A16:F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="B1" s="2"/>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
+      <c r="H2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I8" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="I8" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="5" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="1">
+        <v>2</v>
+      </c>
+      <c r="J11" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="H16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2</v>
+      </c>
+      <c r="E18" s="7">
+        <v>41680.416666666664</v>
+      </c>
+      <c r="F18" s="1">
+        <v>3</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1">
+        <v>2</v>
+      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>2</v>
+      </c>
+      <c r="B19" s="1">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="7">
+        <v>41680.625</v>
+      </c>
+      <c r="F19" s="1">
+        <v>8</v>
+      </c>
+      <c r="H19" s="1">
+        <v>2</v>
+      </c>
+      <c r="I19" s="1">
+        <v>4</v>
+      </c>
+      <c r="J19" s="7">
+        <v>41685.630706018521</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>3</v>
+      </c>
+      <c r="B20" s="1">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="7">
+        <v>41690.416666666664</v>
+      </c>
+      <c r="F20" s="1">
+        <v>5</v>
+      </c>
+      <c r="H20" s="1">
+        <v>3</v>
+      </c>
+      <c r="I20" s="1">
+        <v>5</v>
+      </c>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2</v>
+      </c>
+      <c r="E21" s="7">
+        <v>41685.625</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2</v>
+      </c>
+      <c r="E22" s="7">
+        <v>41695.333333333336</v>
+      </c>
+      <c r="F22" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>